<commit_message>
docs: added a visualization + column to Excel (Python Extensive Course) #53
</commit_message>
<xml_diff>
--- a/docs/assets/python-extensive/data/tabular/fhsstud.xlsx
+++ b/docs/assets/python-extensive/data/tabular/fhsstud.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Lehrgang-Studienanfänge</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Semester</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -478,6 +483,11 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -497,6 +507,11 @@
       <c r="E3" t="n">
         <v>0</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -516,6 +531,11 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -535,6 +555,11 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -554,6 +579,11 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -573,6 +603,11 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -592,6 +627,11 @@
       <c r="E8" t="n">
         <v>0</v>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -611,6 +651,11 @@
       <c r="E9" t="n">
         <v>0</v>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -630,6 +675,11 @@
       <c r="E10" t="n">
         <v>0</v>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -649,6 +699,11 @@
       <c r="E11" t="n">
         <v>0</v>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -668,6 +723,11 @@
       <c r="E12" t="n">
         <v>0</v>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -687,6 +747,11 @@
       <c r="E13" t="n">
         <v>0</v>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -706,6 +771,11 @@
       <c r="E14" t="n">
         <v>427</v>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -725,6 +795,11 @@
       <c r="E15" t="n">
         <v>128</v>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -744,6 +819,11 @@
       <c r="E16" t="n">
         <v>406</v>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -763,6 +843,11 @@
       <c r="E17" t="n">
         <v>232</v>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -782,6 +867,11 @@
       <c r="E18" t="n">
         <v>582</v>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -801,6 +891,11 @@
       <c r="E19" t="n">
         <v>189</v>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -820,6 +915,11 @@
       <c r="E20" t="n">
         <v>536</v>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -839,6 +939,11 @@
       <c r="E21" t="n">
         <v>420</v>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -858,6 +963,11 @@
       <c r="E22" t="n">
         <v>743</v>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -877,6 +987,11 @@
       <c r="E23" t="n">
         <v>369</v>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -896,6 +1011,11 @@
       <c r="E24" t="n">
         <v>934</v>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -915,6 +1035,11 @@
       <c r="E25" t="n">
         <v>501</v>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -934,6 +1059,11 @@
       <c r="E26" t="n">
         <v>1129</v>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -953,6 +1083,11 @@
       <c r="E27" t="n">
         <v>649</v>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -972,6 +1107,11 @@
       <c r="E28" t="n">
         <v>1473</v>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -991,6 +1131,11 @@
       <c r="E29" t="n">
         <v>726</v>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1010,6 +1155,11 @@
       <c r="E30" t="n">
         <v>1802</v>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1029,6 +1179,11 @@
       <c r="E31" t="n">
         <v>870</v>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1048,6 +1203,11 @@
       <c r="E32" t="n">
         <v>1983</v>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1067,6 +1227,11 @@
       <c r="E33" t="n">
         <v>1046</v>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1086,6 +1251,11 @@
       <c r="E34" t="n">
         <v>2230</v>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1105,6 +1275,11 @@
       <c r="E35" t="n">
         <v>1196</v>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1124,6 +1299,11 @@
       <c r="E36" t="n">
         <v>3001</v>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1143,6 +1323,11 @@
       <c r="E37" t="n">
         <v>2045</v>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1162,6 +1347,11 @@
       <c r="E38" t="n">
         <v>3288</v>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1181,6 +1371,11 @@
       <c r="E39" t="n">
         <v>1936</v>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1200,6 +1395,11 @@
       <c r="E40" t="n">
         <v>3747</v>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1219,6 +1419,11 @@
       <c r="E41" t="n">
         <v>2259</v>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1238,6 +1443,11 @@
       <c r="E42" t="n">
         <v>6295</v>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Wintersemester</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1256,6 +1466,11 @@
       </c>
       <c r="E43" t="n">
         <v>884</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Sommersemester</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>